<commit_message>
Uploading image explorer data1, data2, and rules to validator
</commit_message>
<xml_diff>
--- a/code/validator/image_explorer_rules.xlsx
+++ b/code/validator/image_explorer_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\MooreInstitute\Projects\PeoplesLab\Code\Microplastic_Data_Portal\code\validator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4D741BB-68B8-4FC3-A975-87D60F323D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7198331C-813F-4540-A851-E9BB43E7D50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AB5245A-81BA-4195-A22C-D62CA446D157}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{7AB5245A-81BA-4195-A22C-D62CA446D157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>name</t>
   </si>
@@ -59,13 +59,187 @@
     <t>image_file</t>
   </si>
   <si>
-    <t>File Name needs to be unique</t>
-  </si>
-  <si>
     <t>photo.jpg</t>
   </si>
   <si>
     <t>is_unique(ImageFile)</t>
+  </si>
+  <si>
+    <t>image_type</t>
+  </si>
+  <si>
+    <t>researcher_name</t>
+  </si>
+  <si>
+    <t>affiliation</t>
+  </si>
+  <si>
+    <t>citation</t>
+  </si>
+  <si>
+    <t>instrument_name</t>
+  </si>
+  <si>
+    <t>analysis_date</t>
+  </si>
+  <si>
+    <t>polymer_type_of_particle</t>
+  </si>
+  <si>
+    <t>polymer_type_of_particle_original</t>
+  </si>
+  <si>
+    <t>magnification</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>color_original</t>
+  </si>
+  <si>
+    <t>morphology</t>
+  </si>
+  <si>
+    <t>morphology_original</t>
+  </si>
+  <si>
+    <t>size_of_particle</t>
+  </si>
+  <si>
+    <t>size_dimension</t>
+  </si>
+  <si>
+    <t>The full name of the institute where the researcher is from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The researcher's last name and year, which study the image is from, and the full name of the institute where the researcher is from </t>
+  </si>
+  <si>
+    <t>The full name of the instrument</t>
+  </si>
+  <si>
+    <t>The year the image was analyzed</t>
+  </si>
+  <si>
+    <t>The polymer type of the particle or should be an 'NA' if it is unknown</t>
+  </si>
+  <si>
+    <t>The original source of the particle or should be an 'NA' if it is unknown</t>
+  </si>
+  <si>
+    <t>Magnification of the analysis must have an 'x' after the number</t>
+  </si>
+  <si>
+    <t>The color of the particle should be one word with the first letter capitalized, or 'Unknown' if it is not recorded</t>
+  </si>
+  <si>
+    <t>The original color before analysis should be one word with the first letter capitalized, or 'NA' if it is not recorded</t>
+  </si>
+  <si>
+    <t>The morphology of the particle should be one word with the first letter capitalized, or 'NA' if it is not recorded</t>
+  </si>
+  <si>
+    <t>The original morphology before analysis should be one word with the first letter capitalized, or 'NA' if it is not recorded</t>
+  </si>
+  <si>
+    <t>The size of the particle should have a unit after the number and can be a range</t>
+  </si>
+  <si>
+    <t>The name of the size used to describe the plastic rather than the exact dimensions</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>Charles Moore and Gwen Lattin</t>
+  </si>
+  <si>
+    <t>Moore Institute for Plastic Pollution Research</t>
+  </si>
+  <si>
+    <t>Lattin and Moore 2020, Interlab Comparison Study Data, Moore Institute for Plastic Pollution Research</t>
+  </si>
+  <si>
+    <t>Nikon SMZ1270</t>
+  </si>
+  <si>
+    <t>7-10x</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>The first and last name of the researcher or the name of the lab</t>
+  </si>
+  <si>
+    <t>Organic Matter</t>
+  </si>
+  <si>
+    <t>Fiber</t>
+  </si>
+  <si>
+    <t>20-212 um</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t>is.character(researcher_name)</t>
+  </si>
+  <si>
+    <t>is.character(affiliation)</t>
+  </si>
+  <si>
+    <t>File name needs to be unique</t>
+  </si>
+  <si>
+    <t>!is.na(analysis_date) &amp; grep1("^\\d{4}(-\\d{4})?$", analysis_date)</t>
+  </si>
+  <si>
+    <t>is.character(magnification) &amp; grep1("^\\d+-\\d+x$|^NA$", magnification)</t>
+  </si>
+  <si>
+    <t>is.character(size_of_particle) &amp; grep1("^\\d+-\\d+ um$|^&gt;\\d+ um$|^NA$", size_of_particle)</t>
+  </si>
+  <si>
+    <t>size_dimension %in% c("Nominal", "nominal")</t>
+  </si>
+  <si>
+    <t>ImageType %in% c("SEM", "Visual", "Fluorescence")</t>
+  </si>
+  <si>
+    <t>Image type should be SEM, Visual, or Fluorescence</t>
+  </si>
+  <si>
+    <t>color %in% c("Green", "White", "Black", "Transparent", "Pink", "Blue", "Grey", "Purple", "Red", "Yellow", "Orange", "Brown", "Other", "Unknown")</t>
+  </si>
+  <si>
+    <t>color_original %in% c("Green", "White", "Black", "Transparent", "Pink", "Blue", "Grey", "Purple", "Red", "Yellow", "Orange", "Brown", "Other", "Unknown")</t>
+  </si>
+  <si>
+    <t>morphology %in% c("Sphere", "Film", "Fiber", "Fragment", "Foam", "Fiber Bundle", "Bead", "Nurdle", "NA")</t>
+  </si>
+  <si>
+    <t>morphology_original %in% c("Sphere", "Film", "Fiber", "Fragment", "Foam", "Fiber Bundle", "Bead", "Nurdle", "NA")</t>
+  </si>
+  <si>
+    <t>warning</t>
+  </si>
+  <si>
+    <t>instrument_name %in% c("Nikon SMZ1270", "NA", "MEIJI TECHNO EMZ-8TR with OptixCAM summit K2", "Olympus MVX-ZB10")</t>
+  </si>
+  <si>
+    <t>is.character(citation)</t>
+  </si>
+  <si>
+    <t>polymer_type_of_particle %in% c("NA", "Polyethylene", "Polystyrene", "Nylon", "Polypropylene", "Organic Matter", "Other Plastic", "PE", "PS", "cellulose", "PET", "PVC", "Mineral")</t>
+  </si>
+  <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>polymer_type_of_particle_original %in% c("NA", "Polyethylene", "Polystyrene", "Nylon", "Polypropylene", "Organic Matter", "Other Plastic", "PE", "PS", "cellulose", "PET", "PVC", "Mineral", "cotton")</t>
   </si>
 </sst>
 </file>
@@ -101,8 +275,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,15 +592,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5893CA-AEB2-4268-BDF3-93BA9258DF5B}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,21 +615,276 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>2020</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code validator rules
</commit_message>
<xml_diff>
--- a/code/validator/image_explorer_rules.xlsx
+++ b/code/validator/image_explorer_rules.xlsx
@@ -5,21 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7198331C-813F-4540-A851-E9BB43E7D50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FE07950-9E42-4A44-9665-6923C6A0A121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{7AB5245A-81BA-4195-A22C-D62CA446D157}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="image_explorer_rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -110,42 +107,12 @@
     <t>size_dimension</t>
   </si>
   <si>
-    <t>The full name of the institute where the researcher is from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The researcher's last name and year, which study the image is from, and the full name of the institute where the researcher is from </t>
-  </si>
-  <si>
     <t>The full name of the instrument</t>
   </si>
   <si>
     <t>The year the image was analyzed</t>
   </si>
   <si>
-    <t>The polymer type of the particle or should be an 'NA' if it is unknown</t>
-  </si>
-  <si>
-    <t>The original source of the particle or should be an 'NA' if it is unknown</t>
-  </si>
-  <si>
-    <t>Magnification of the analysis must have an 'x' after the number</t>
-  </si>
-  <si>
-    <t>The color of the particle should be one word with the first letter capitalized, or 'Unknown' if it is not recorded</t>
-  </si>
-  <si>
-    <t>The original color before analysis should be one word with the first letter capitalized, or 'NA' if it is not recorded</t>
-  </si>
-  <si>
-    <t>The morphology of the particle should be one word with the first letter capitalized, or 'NA' if it is not recorded</t>
-  </si>
-  <si>
-    <t>The original morphology before analysis should be one word with the first letter capitalized, or 'NA' if it is not recorded</t>
-  </si>
-  <si>
-    <t>The size of the particle should have a unit after the number and can be a range</t>
-  </si>
-  <si>
     <t>The name of the size used to describe the plastic rather than the exact dimensions</t>
   </si>
   <si>
@@ -170,9 +137,6 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>The first and last name of the researcher or the name of the lab</t>
-  </si>
-  <si>
     <t>Organic Matter</t>
   </si>
   <si>
@@ -185,61 +149,94 @@
     <t>Nominal</t>
   </si>
   <si>
-    <t>is.character(researcher_name)</t>
-  </si>
-  <si>
-    <t>is.character(affiliation)</t>
-  </si>
-  <si>
     <t>File name needs to be unique</t>
   </si>
   <si>
-    <t>!is.na(analysis_date) &amp; grep1("^\\d{4}(-\\d{4})?$", analysis_date)</t>
-  </si>
-  <si>
-    <t>is.character(magnification) &amp; grep1("^\\d+-\\d+x$|^NA$", magnification)</t>
-  </si>
-  <si>
-    <t>is.character(size_of_particle) &amp; grep1("^\\d+-\\d+ um$|^&gt;\\d+ um$|^NA$", size_of_particle)</t>
-  </si>
-  <si>
-    <t>size_dimension %in% c("Nominal", "nominal")</t>
-  </si>
-  <si>
-    <t>ImageType %in% c("SEM", "Visual", "Fluorescence")</t>
-  </si>
-  <si>
     <t>Image type should be SEM, Visual, or Fluorescence</t>
   </si>
   <si>
-    <t>color %in% c("Green", "White", "Black", "Transparent", "Pink", "Blue", "Grey", "Purple", "Red", "Yellow", "Orange", "Brown", "Other", "Unknown")</t>
-  </si>
-  <si>
-    <t>color_original %in% c("Green", "White", "Black", "Transparent", "Pink", "Blue", "Grey", "Purple", "Red", "Yellow", "Orange", "Brown", "Other", "Unknown")</t>
-  </si>
-  <si>
-    <t>morphology %in% c("Sphere", "Film", "Fiber", "Fragment", "Foam", "Fiber Bundle", "Bead", "Nurdle", "NA")</t>
-  </si>
-  <si>
-    <t>morphology_original %in% c("Sphere", "Film", "Fiber", "Fragment", "Foam", "Fiber Bundle", "Bead", "Nurdle", "NA")</t>
-  </si>
-  <si>
     <t>warning</t>
   </si>
   <si>
-    <t>instrument_name %in% c("Nikon SMZ1270", "NA", "MEIJI TECHNO EMZ-8TR with OptixCAM summit K2", "Olympus MVX-ZB10")</t>
-  </si>
-  <si>
-    <t>is.character(citation)</t>
-  </si>
-  <si>
-    <t>polymer_type_of_particle %in% c("NA", "Polyethylene", "Polystyrene", "Nylon", "Polypropylene", "Organic Matter", "Other Plastic", "PE", "PS", "cellulose", "PET", "PVC", "Mineral")</t>
-  </si>
-  <si>
     <t>cotton</t>
   </si>
   <si>
-    <t>polymer_type_of_particle_original %in% c("NA", "Polyethylene", "Polystyrene", "Nylon", "Polypropylene", "Organic Matter", "Other Plastic", "PE", "PS", "cellulose", "PET", "PVC", "Mineral", "cotton")</t>
+    <t>Morphology %in% c("Sphere", "Film", "Fiber", "Fragment", "Foam", "Fiber Bundle", "Bead", "Nurdle", "NA")</t>
+  </si>
+  <si>
+    <t>Magnification of the analysis must be written as a number or with an 'x' after</t>
+  </si>
+  <si>
+    <t>is.character(Magnification) &amp; grepl("^\\d+-\\d+x$|^\\d+x$|^\\d+$|^NA$", Magnification)</t>
+  </si>
+  <si>
+    <t>!is.na(AnalysisDate) &amp; grepl("^\\d{4}(-\\d{4})?$", AnalysisDate)</t>
+  </si>
+  <si>
+    <t>The polymer of the particle should fit within one of these categories: NA, Polyethylene, Polystyrene, Nylon, Polypropylene, Organic Matter, Other Plastic, PE, PS, cellulose, PET, PVC, Mineral</t>
+  </si>
+  <si>
+    <t>The color of the particle should fit within one of these categories: Green, White, Black, Transparent, Pink, Blue, Grey, Purple, Red, Yellow, Orange, Brown, Other, Unknown</t>
+  </si>
+  <si>
+    <t>The morphology of the particle should fit within one of these categories: Sphere, Film, Fiber, Fragment, Foam, Fiber Bundle, Bead, Nurdle, NA</t>
+  </si>
+  <si>
+    <t>The size of the particle should fit within one of these size classes: &gt;500 um, 20-212 um, 1-20 um, 212-500 um, &lt;500 um, 50-250 um, &gt;1 mm, 100-500um, 1.5mm, &gt;500, &gt;3mm, ~2mm, ~1mm, 2mm, 3mm, ~3mm, &gt;500um, NA</t>
+  </si>
+  <si>
+    <t>InstrumentName %in% c("Nikon SMZ1270", "NA", "MEIJI TECHNO EMZ-8TR with OptixCAM summit K2", "Olympus MVX-ZB10")</t>
+  </si>
+  <si>
+    <t>PolymerTypeOfParticle %in% c("NA", "Polyethylene", "Polystyrene", "Nylon", "Polypropylene", "Organic Matter", "Other Plastic", "PE", "PS", "cellulose", "PET", "PVC", "Mineral")</t>
+  </si>
+  <si>
+    <t>SizeOfParticle %in% c("&gt;500 um", "20-212 um", "1-20 um", "212-500 um", "&lt;500 um", "50-250 um", "&gt;1 mm", "100-500um", "1.5mm", "&gt;500", "&gt;3mm", "~2mm", "~1mm", "2mm", "3mm", "~3mm", "&gt;500um", "NA")</t>
+  </si>
+  <si>
+    <t>The name of the researcher or the name of the lab must not be an 'NA'</t>
+  </si>
+  <si>
+    <t>The name of the institute where the researcher is from must not be an 'NA'</t>
+  </si>
+  <si>
+    <t>The citation must not be an 'NA'</t>
+  </si>
+  <si>
+    <t>!is.na(ResearcherName)</t>
+  </si>
+  <si>
+    <t>!is.na(Affiliation)</t>
+  </si>
+  <si>
+    <t>!is.na(Citation)</t>
+  </si>
+  <si>
+    <t>PolymerTypeOfParticleOriginal %in% c("NA", "Polyethylene", "Polystyrene", "Nylon", "Polypropylene", "Organic Matter", "Other Plastic", "PE", "PS", "cellulose", "PET", "PVC", "Mineral")</t>
+  </si>
+  <si>
+    <t>ColorOriginal %in% c("Green", "White", "Black", "Transparent", "Pink", "Blue", "Grey", "Purple", "Red", "Yellow", "Orange", "Brown", "Other", "Unknown")</t>
+  </si>
+  <si>
+    <t>MorphologyOriginal %in% c("Sphere", "Film", "Fiber", "Fragment", "Foam", "Fiber Bundle", "Bead", "Nurdle", "NA")</t>
+  </si>
+  <si>
+    <t>If the original polymer type is not within the polymer categories, it will appear as a warning</t>
+  </si>
+  <si>
+    <t>If the original color is not within one of the color categories, it will appear as a warning</t>
+  </si>
+  <si>
+    <t>If the original morphology is not within one of the morphology categories, it will appear as a warning</t>
+  </si>
+  <si>
+    <t>SizeDimension %in% c("Nominal", "nominal", "ferret diameter", "longest length") &amp; !is.na(SizeDimension)</t>
+  </si>
+  <si>
+    <t>Color %in% c("Green", "White", "Black", "Transparent", "Pink", "Blue", "Grey", "Purple", "Red", "Yellow", "Orange", "Brown", "Other", "Unknown") &amp; !is.na(Color)</t>
+  </si>
+  <si>
+    <t>ImageType %in% c("SEM", "Visual", "Fluorescence") &amp; !is.na(ImageType)</t>
   </si>
 </sst>
 </file>
@@ -275,9 +272,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +587,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5893CA-AEB2-4268-BDF3-93BA9258DF5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -620,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -633,20 +631,20 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -654,16 +652,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -671,16 +669,16 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -688,16 +686,16 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -705,16 +703,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -722,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>2020</v>
@@ -731,7 +729,7 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -739,16 +737,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -756,16 +754,16 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -773,16 +771,16 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -790,16 +788,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -807,16 +805,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -824,16 +822,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -841,13 +839,13 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
         <v>61</v>
@@ -858,16 +856,16 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -875,16 +873,16 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>